<commit_message>
UTS PERBAIKAN (Tambah Detail Penjualan)
</commit_message>
<xml_diff>
--- a/public/template_penjualan.xlsx
+++ b/public/template_penjualan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS_2024\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98F39E24-DA42-40ED-AD85-6D4120AFD359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1852D1-A2CA-4C6C-8657-087B7275A5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{026C1130-9F5A-4CD3-9807-C979A1EC8352}"/>
+    <workbookView xWindow="2340" yWindow="855" windowWidth="10365" windowHeight="10665" xr2:uid="{026C1130-9F5A-4CD3-9807-C979A1EC8352}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -34,40 +34,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>pembeli</t>
-  </si>
-  <si>
-    <t>penjualan_kode</t>
-  </si>
-  <si>
-    <t>penjualan_tanggal</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>TRX011</t>
-  </si>
-  <si>
-    <t>24-10-2024</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Kode Transaksi</t>
+  </si>
+  <si>
+    <t>Barang</t>
+  </si>
+  <si>
+    <t>Harga</t>
+  </si>
+  <si>
+    <t>Jumlah</t>
+  </si>
+  <si>
+    <t>TRX001</t>
+  </si>
+  <si>
+    <t>Chitato</t>
+  </si>
+  <si>
+    <t>Beef Slice</t>
+  </si>
+  <si>
+    <t>Indomilk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,11 +96,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -118,7 +116,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -414,37 +412,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37827B0-5B98-4ED2-A7B4-017FEBF2E8E5}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="19.21875" customWidth="1"/>
+    <col min="2" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>25000</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>6500</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>